<commit_message>
add models to all biorefineries
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/wwt/results/oc1g_exist_uncertainties.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/wwt/results/oc1g_exist_uncertainties.xlsx
@@ -516,72 +516,72 @@
       <c r="G1" s="1" t="n"/>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Stream-catalyst</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-biodiesel wash water</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-HCl</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-NaOH</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-oilcane</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-denaturant</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-methanol</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Stream-s154</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Stream-s155</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Stream-lime</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Stream-acetone</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Stream-pure glycerine</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Stream-cooling tower chemicals</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Stream-makeup water</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-methanol</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-catalyst</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-biodiesel wash water</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-HCl</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-NaOH</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-oilcane</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-denaturant</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
@@ -654,72 +654,72 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
+          <t>Catalyst price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Biodiesel wash water price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>HCl price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>Na OH price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>Oilcane price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>Denaturant price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>Methanol price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
           <t>S154 price [USD/kg]</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>S155 price [USD/kg]</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>Lime price [USD/kg]</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>Acetone price [USD/kg]</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="S2" s="1" t="inlineStr">
         <is>
           <t>Pure glycerine price [USD/kg]</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>Cooling tower chemicals price [USD/kg]</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>Makeup water price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>Methanol price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>Catalyst price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>Biodiesel wash water price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="R2" s="1" t="inlineStr">
-        <is>
-          <t>HCl price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="S2" s="1" t="inlineStr">
-        <is>
-          <t>Na OH price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="T2" s="1" t="inlineStr">
-        <is>
-          <t>Oilcane price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="U2" s="1" t="inlineStr">
-        <is>
-          <t>Denaturant price [USD/kg]</t>
         </is>
       </c>
       <c r="V2" s="1" t="inlineStr">
@@ -763,85 +763,85 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>357932.6012637048</v>
+        <v>319933.8791364545</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8050793421093427</v>
+        <v>0.8786644138052185</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9473563265903202</v>
+        <v>0.8871937031661965</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7405554300604852</v>
+        <v>0.7547278197304041</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8177556382943275</v>
+        <v>0.8052815644220522</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8848171238933005</v>
+        <v>0.8489016030834337</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2304649160473426</v>
+        <v>3.371083913010652</v>
       </c>
       <c r="I4" t="n">
-        <v>4.018721223551006</v>
+        <v>0.0003606812768118197</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06687066685588682</v>
+        <v>0.07410749344466867</v>
       </c>
       <c r="K4" t="n">
-        <v>0.939339977825246</v>
+        <v>0.4552178678269928</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6707046980773463</v>
+        <v>0.0353641481148252</v>
       </c>
       <c r="M4" t="n">
-        <v>2.866617665688383</v>
+        <v>0.8826563199816162</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0002500360999305225</v>
+        <v>0.6522672418471019</v>
       </c>
       <c r="O4" t="n">
-        <v>0.6463647004946969</v>
+        <v>0.1959209426376695</v>
       </c>
       <c r="P4" t="n">
-        <v>2.77165469984371</v>
+        <v>5.470272573962804</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0004009528610403349</v>
+        <v>0.08649226948631465</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0751299091857897</v>
+        <v>0.789789487261971</v>
       </c>
       <c r="S4" t="n">
-        <v>0.3446022514793721</v>
+        <v>0.7068668259051389</v>
       </c>
       <c r="T4" t="n">
-        <v>0.03273125844191845</v>
+        <v>3.40564778091172</v>
       </c>
       <c r="U4" t="n">
-        <v>0.7991714146296076</v>
+        <v>0.0002530966049521194</v>
       </c>
       <c r="V4" t="n">
-        <v>0.6878961757376787</v>
+        <v>0.6063536285641343</v>
       </c>
       <c r="W4" t="n">
-        <v>1.253519514243771</v>
+        <v>1.140441508435972</v>
       </c>
       <c r="X4" t="n">
-        <v>0.1707587393208577</v>
+        <v>0.1432311571221447</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.05698111291165429</v>
+        <v>0.07089763418581578</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.5780738828464115</v>
+        <v>0.6234441682918634</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.694883026479991</v>
+        <v>0.628306728617419</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.03688387115176386</v>
+        <v>-0.03191340379370473</v>
       </c>
     </row>
     <row r="5">
@@ -849,85 +849,85 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>380874.5579471973</v>
+        <v>313564.8105574455</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8848928661378663</v>
+        <v>0.7998684796327056</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6946711890489051</v>
+        <v>0.7244969015158683</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8840091028660189</v>
+        <v>0.8322339575776623</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8294670072924083</v>
+        <v>0.7999660034436795</v>
       </c>
       <c r="G5" t="n">
-        <v>0.84641421771937</v>
+        <v>0.8830702141683747</v>
       </c>
       <c r="H5" t="n">
-        <v>0.21422386968229</v>
+        <v>2.743042574648345</v>
       </c>
       <c r="I5" t="n">
-        <v>5.890321925513112</v>
+        <v>0.0003289364024939061</v>
       </c>
       <c r="J5" t="n">
-        <v>0.08299128037592571</v>
+        <v>0.07687303024649192</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9082071720196501</v>
+        <v>0.3300847609639892</v>
       </c>
       <c r="L5" t="n">
-        <v>0.6556124558378787</v>
+        <v>0.03220473282091099</v>
       </c>
       <c r="M5" t="n">
-        <v>3.067923688148006</v>
+        <v>0.6227138591153392</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0002762051863299435</v>
+        <v>0.5403375284695384</v>
       </c>
       <c r="O5" t="n">
-        <v>0.6149568146394602</v>
+        <v>0.2189978976353245</v>
       </c>
       <c r="P5" t="n">
-        <v>3.505156157978153</v>
+        <v>4.878687567321744</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0003531316033044186</v>
+        <v>0.07119481577661639</v>
       </c>
       <c r="R5" t="n">
-        <v>0.07861538951185934</v>
+        <v>0.6684021898548804</v>
       </c>
       <c r="S5" t="n">
-        <v>0.3582513665714649</v>
+        <v>0.5583616497817865</v>
       </c>
       <c r="T5" t="n">
-        <v>0.03854801717921231</v>
+        <v>2.397484135322718</v>
       </c>
       <c r="U5" t="n">
-        <v>0.826881623507433</v>
+        <v>0.0002973096862628245</v>
       </c>
       <c r="V5" t="n">
-        <v>0.6126337564797641</v>
+        <v>0.6235737575200697</v>
       </c>
       <c r="W5" t="n">
-        <v>1.171157103863737</v>
+        <v>1.124533060291984</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1666614805182885</v>
+        <v>0.1617178972468668</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.06841455172905073</v>
+        <v>0.07677557266839527</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.4117509574256206</v>
+        <v>0.4296267132280529</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.6548330429996689</v>
+        <v>0.5633296252026652</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.02396246450497103</v>
+        <v>-0.03673171780419767</v>
       </c>
     </row>
     <row r="6">
@@ -935,85 +935,85 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>339464.7892672957</v>
+        <v>298652.536961208</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8749111178413539</v>
+        <v>0.913598896791175</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7116653946998395</v>
+        <v>0.943496240823478</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9517411438805221</v>
+        <v>0.9113945443861972</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7336412871831807</v>
+        <v>0.8367900742233263</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9063845158144797</v>
+        <v>0.9050128317595117</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2005501439903596</v>
+        <v>2.428895133991007</v>
       </c>
       <c r="I6" t="n">
-        <v>4.437146399598171</v>
+        <v>0.0003349395669201685</v>
       </c>
       <c r="J6" t="n">
-        <v>0.07672740599443309</v>
+        <v>0.06535896488265164</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6448483237247977</v>
+        <v>0.3718497468777013</v>
       </c>
       <c r="L6" t="n">
-        <v>0.6263909441650932</v>
+        <v>0.03077571193578649</v>
       </c>
       <c r="M6" t="n">
-        <v>2.539087679486212</v>
+        <v>0.7339930552387709</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0002352699943945606</v>
+        <v>0.5626895778130635</v>
       </c>
       <c r="O6" t="n">
-        <v>0.5812744007026547</v>
+        <v>0.1865517132625418</v>
       </c>
       <c r="P6" t="n">
-        <v>2.38668863019183</v>
+        <v>4.455897444275112</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0003255906676568453</v>
+        <v>0.06673526631902278</v>
       </c>
       <c r="R6" t="n">
-        <v>0.07780260776090593</v>
+        <v>0.826143511831454</v>
       </c>
       <c r="S6" t="n">
-        <v>0.4693862935235245</v>
+        <v>0.7296670527853253</v>
       </c>
       <c r="T6" t="n">
-        <v>0.03240840898660156</v>
+        <v>2.921417212231451</v>
       </c>
       <c r="U6" t="n">
-        <v>0.7267467288232681</v>
+        <v>0.0002203378486013878</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7253610850711051</v>
+        <v>0.5711303623513122</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8611082579166746</v>
+        <v>1.337108941149416</v>
       </c>
       <c r="X6" t="n">
-        <v>0.157516751009419</v>
+        <v>0.1473001313631098</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.06067101652561339</v>
+        <v>0.04973075899074028</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.5903749241971649</v>
+        <v>0.4369975314761926</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.5215313297916584</v>
+        <v>0.5239575505479821</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.02533049424388528</v>
+        <v>-0.02503493230972102</v>
       </c>
     </row>
     <row r="7">
@@ -1021,85 +1021,85 @@
         <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>306651.6496836966</v>
+        <v>373253.3617076025</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9483675794212933</v>
+        <v>0.9615925260144773</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8662597510003653</v>
+        <v>0.9166889648538187</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8490271008094838</v>
+        <v>0.9486240135092125</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7742700633634951</v>
+        <v>0.7723284792010902</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8770973509454676</v>
+        <v>0.8183695922241495</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1892556229235258</v>
+        <v>2.888508906946005</v>
       </c>
       <c r="I7" t="n">
-        <v>5.304103991257275</v>
+        <v>0.0003521331319636663</v>
       </c>
       <c r="J7" t="n">
-        <v>0.08108096161014949</v>
+        <v>0.06149890043060448</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7906268219097432</v>
+        <v>0.4007447454966814</v>
       </c>
       <c r="L7" t="n">
-        <v>0.7049946873095743</v>
+        <v>0.03749849115362162</v>
       </c>
       <c r="M7" t="n">
-        <v>3.29781953084454</v>
+        <v>0.7371042881218192</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0002785990496345957</v>
+        <v>0.5539201297055767</v>
       </c>
       <c r="O7" t="n">
-        <v>0.5506236888700741</v>
+        <v>0.2006651951209002</v>
       </c>
       <c r="P7" t="n">
-        <v>2.535191236107107</v>
+        <v>5.17705000214424</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0003156966645211407</v>
+        <v>0.07554682695622253</v>
       </c>
       <c r="R7" t="n">
-        <v>0.06823077024195216</v>
+        <v>0.7072223399099908</v>
       </c>
       <c r="S7" t="n">
-        <v>0.3836085530734214</v>
+        <v>0.6250222003260829</v>
       </c>
       <c r="T7" t="n">
-        <v>0.04058299123724349</v>
+        <v>2.693368682757011</v>
       </c>
       <c r="U7" t="n">
-        <v>0.7785495170741203</v>
+        <v>0.0002432283270730846</v>
       </c>
       <c r="V7" t="n">
-        <v>0.702566135301615</v>
+        <v>0.6707481097186991</v>
       </c>
       <c r="W7" t="n">
-        <v>1.056249536722339</v>
+        <v>1.22594003824971</v>
       </c>
       <c r="X7" t="n">
-        <v>0.1480772555405145</v>
+        <v>0.1737448321091259</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.07186591905146845</v>
+        <v>0.06582908898554571</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.5490981127761296</v>
+        <v>0.6520917483703238</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.5634543443433764</v>
+        <v>0.614031479278348</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.03335754274654502</v>
+        <v>-0.03121978261009316</v>
       </c>
     </row>
     <row r="8">
@@ -1107,85 +1107,85 @@
         <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>262514.6472840727</v>
+        <v>281680.2219344516</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9776222478985327</v>
+        <v>0.9969116463250449</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7509482924711647</v>
+        <v>0.8595948980231926</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9255614997637419</v>
+        <v>0.7994477860400596</v>
       </c>
       <c r="F8" t="n">
-        <v>0.762761199003973</v>
+        <v>0.808929405160542</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8004565699820949</v>
+        <v>0.7915694994022243</v>
       </c>
       <c r="H8" t="n">
-        <v>0.222414628104058</v>
+        <v>2.965343095009235</v>
       </c>
       <c r="I8" t="n">
-        <v>4.858549629553575</v>
+        <v>0.0003698078739804615</v>
       </c>
       <c r="J8" t="n">
-        <v>0.07346495704723242</v>
+        <v>0.07060588205798324</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8383980380237968</v>
+        <v>0.3858916738723712</v>
       </c>
       <c r="L8" t="n">
-        <v>0.5013976616738217</v>
+        <v>0.03317278914125589</v>
       </c>
       <c r="M8" t="n">
-        <v>2.811651265696538</v>
+        <v>0.7709245333954597</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0002614183494726501</v>
+        <v>0.5072953946658069</v>
       </c>
       <c r="O8" t="n">
-        <v>0.5138991706686693</v>
+        <v>0.2478154060836067</v>
       </c>
       <c r="P8" t="n">
-        <v>3.223722110428652</v>
+        <v>4.154164732492569</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.000374478451998614</v>
+        <v>0.09144690280952712</v>
       </c>
       <c r="R8" t="n">
-        <v>0.07166848239099474</v>
+        <v>0.7463118804327451</v>
       </c>
       <c r="S8" t="n">
-        <v>0.4072027635374821</v>
+        <v>0.6565684310540738</v>
       </c>
       <c r="T8" t="n">
-        <v>0.02699802592531141</v>
+        <v>2.804626114575094</v>
       </c>
       <c r="U8" t="n">
-        <v>0.7653313531650924</v>
+        <v>0.000198263257584019</v>
       </c>
       <c r="V8" t="n">
-        <v>0.6677690295363166</v>
+        <v>0.7124049616723603</v>
       </c>
       <c r="W8" t="n">
-        <v>1.042586632760334</v>
+        <v>1.093486639699995</v>
       </c>
       <c r="X8" t="n">
-        <v>0.151808114866478</v>
+        <v>0.1652754070604397</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.05851927416908165</v>
+        <v>0.05914527682491581</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.444357116852826</v>
+        <v>0.5778473413310297</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.6767308840556633</v>
+        <v>0.6508017048837519</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.02665573302878534</v>
+        <v>-0.02602294793059929</v>
       </c>
     </row>
     <row r="9">
@@ -1193,85 +1193,85 @@
         <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>374835.9216336525</v>
+        <v>400402.9982207899</v>
       </c>
       <c r="C9" t="n">
-        <v>0.96345743369695</v>
+        <v>0.8443328418904813</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7976356757661157</v>
+        <v>0.7438957710474825</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8212491308656801</v>
+        <v>0.8594039968340557</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7981961958628567</v>
+        <v>0.7461817695488248</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8351630490737511</v>
+        <v>0.833700452055553</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1847439318249173</v>
+        <v>3.17804860258555</v>
       </c>
       <c r="I9" t="n">
-        <v>4.601013982454439</v>
+        <v>0.0003892960700962455</v>
       </c>
       <c r="J9" t="n">
-        <v>0.07005841816291634</v>
+        <v>0.07959573339432315</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7541013758032719</v>
+        <v>0.4123240968521634</v>
       </c>
       <c r="L9" t="n">
-        <v>0.7597633661141168</v>
+        <v>0.0404902691028737</v>
       </c>
       <c r="M9" t="n">
-        <v>3.443838137939585</v>
+        <v>0.7124796148590791</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0002936131766009249</v>
+        <v>0.5831842329375594</v>
       </c>
       <c r="O9" t="n">
-        <v>0.4312023970755172</v>
+        <v>0.1928873412831012</v>
       </c>
       <c r="P9" t="n">
-        <v>2.938731695466159</v>
+        <v>5.416343020792297</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0003480708247751944</v>
+        <v>0.07344880365788668</v>
       </c>
       <c r="R9" t="n">
-        <v>0.06694034404471129</v>
+        <v>0.9156469590806386</v>
       </c>
       <c r="S9" t="n">
-        <v>0.4352197954596095</v>
+        <v>0.7550472805697284</v>
       </c>
       <c r="T9" t="n">
-        <v>0.03365331171496774</v>
+        <v>3.217569490505013</v>
       </c>
       <c r="U9" t="n">
-        <v>0.6153240920929001</v>
+        <v>0.0002313902238183701</v>
       </c>
       <c r="V9" t="n">
-        <v>0.5162034309052904</v>
+        <v>0.5121386256421967</v>
       </c>
       <c r="W9" t="n">
-        <v>1.108924586452716</v>
+        <v>0.9846438667994801</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1450744958004219</v>
+        <v>0.1546985354806635</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.06346109196674382</v>
+        <v>0.06807566730984353</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.4648285702398428</v>
+        <v>0.5410149077664257</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.6244501301952565</v>
+        <v>0.5964974973357967</v>
       </c>
       <c r="AB9" t="n">
-        <v>-0.0288528336010218</v>
+        <v>-0.0351770958973858</v>
       </c>
     </row>
     <row r="10">
@@ -1279,85 +1279,85 @@
         <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>319102.759530023</v>
+        <v>351175.8106339728</v>
       </c>
       <c r="C10" t="n">
-        <v>0.900334206541735</v>
+        <v>0.8697762383658201</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9917626146810653</v>
+        <v>0.8182754452483054</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9774766061836527</v>
+        <v>0.7013345707951792</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8206141369524137</v>
+        <v>0.7578739986428953</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8174669755169829</v>
+        <v>0.8593642329489898</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1749728632329005</v>
+        <v>2.638420686539074</v>
       </c>
       <c r="I10" t="n">
-        <v>5.640251850759157</v>
+        <v>0.0003196245252555553</v>
       </c>
       <c r="J10" t="n">
-        <v>0.06409775651586852</v>
+        <v>0.06894728972837243</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8506783990961555</v>
+        <v>0.4315126165352834</v>
       </c>
       <c r="L10" t="n">
-        <v>0.7207662411245863</v>
+        <v>0.03834731055504404</v>
       </c>
       <c r="M10" t="n">
-        <v>2.695074613041329</v>
+        <v>0.795378220251483</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0002271947735975387</v>
+        <v>0.4489860102373564</v>
       </c>
       <c r="O10" t="n">
-        <v>0.4739654241589719</v>
+        <v>0.2090332745895152</v>
       </c>
       <c r="P10" t="n">
-        <v>2.895101327008005</v>
+        <v>5.019382691916063</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.0003422122621223608</v>
+        <v>0.07707060939494925</v>
       </c>
       <c r="R10" t="n">
-        <v>0.05850898993652914</v>
+        <v>0.768428041134154</v>
       </c>
       <c r="S10" t="n">
-        <v>0.4567708065267042</v>
+        <v>0.6807928507109652</v>
       </c>
       <c r="T10" t="n">
-        <v>0.03611581549339146</v>
+        <v>3.492202002166365</v>
       </c>
       <c r="U10" t="n">
-        <v>0.7499256611090723</v>
+        <v>0.0002691924648784527</v>
       </c>
       <c r="V10" t="n">
-        <v>0.5712623011318159</v>
+        <v>0.5865003479315394</v>
       </c>
       <c r="W10" t="n">
-        <v>1.087289938140449</v>
+        <v>1.013203054986206</v>
       </c>
       <c r="X10" t="n">
-        <v>0.1850441239581416</v>
+        <v>0.1593809587985065</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.0526963008505729</v>
+        <v>0.05553158358841925</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.6933977555140731</v>
+        <v>0.5981087897930929</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.6060014142635686</v>
+        <v>0.6893331415071603</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.03480064746924984</v>
+        <v>-0.02393852033030601</v>
       </c>
     </row>
     <row r="11">
@@ -1365,85 +1365,85 @@
         <v>7</v>
       </c>
       <c r="B11" t="n">
-        <v>299040.5542209736</v>
+        <v>337659.3293759496</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7966365430890057</v>
+        <v>0.7736179346218206</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8348915746762982</v>
+        <v>0.9973860093723005</v>
       </c>
       <c r="E11" t="n">
-        <v>0.684490276926683</v>
+        <v>0.9972793057091298</v>
       </c>
       <c r="F11" t="n">
-        <v>0.867094504336779</v>
+        <v>0.8219447735447114</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8528564833821041</v>
+        <v>0.8747207804720781</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1958610414348189</v>
+        <v>3.240585565110913</v>
       </c>
       <c r="I11" t="n">
-        <v>4.884598240308491</v>
+        <v>0.0004200628429911011</v>
       </c>
       <c r="J11" t="n">
-        <v>0.08610130316578292</v>
+        <v>0.07327363422485261</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8002623188850734</v>
+        <v>0.4386008280703952</v>
       </c>
       <c r="L11" t="n">
-        <v>0.576485939601547</v>
+        <v>0.03594314236113292</v>
       </c>
       <c r="M11" t="n">
-        <v>2.93649508044741</v>
+        <v>0.662310983551104</v>
       </c>
       <c r="N11" t="n">
-        <v>0.000247186030009474</v>
+        <v>0.6024099123734256</v>
       </c>
       <c r="O11" t="n">
-        <v>0.5418198638264584</v>
+        <v>0.159822979639685</v>
       </c>
       <c r="P11" t="n">
-        <v>3.172639721840791</v>
+        <v>4.827616848356666</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0003715558475813992</v>
+        <v>0.06540690132546848</v>
       </c>
       <c r="R11" t="n">
-        <v>0.08536282500207992</v>
+        <v>0.8046943861715045</v>
       </c>
       <c r="S11" t="n">
-        <v>0.3950506301802912</v>
+        <v>0.6471059832167992</v>
       </c>
       <c r="T11" t="n">
-        <v>0.03063638760737266</v>
+        <v>3.116009606296744</v>
       </c>
       <c r="U11" t="n">
-        <v>0.8967484793597706</v>
+        <v>0.000254807598542642</v>
       </c>
       <c r="V11" t="n">
-        <v>0.6317349260299548</v>
+        <v>0.6400406371680076</v>
       </c>
       <c r="W11" t="n">
-        <v>1.285812441949361</v>
+        <v>0.8757355991885388</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1631159534491266</v>
+        <v>0.1802062198730517</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.06597089756153006</v>
+        <v>0.06237778198822949</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.5019972760358175</v>
+        <v>0.6796867243162839</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.517959691355853</v>
+        <v>0.5455972242559897</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.03016929260170088</v>
+        <v>-0.02764856853801772</v>
       </c>
     </row>
     <row r="12">
@@ -1451,85 +1451,85 @@
         <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>347404.9526774819</v>
+        <v>353922.3490579935</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7526196013002304</v>
+        <v>0.94378634000099</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9124882691678078</v>
+        <v>0.6941703842129278</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7255248407727003</v>
+        <v>0.7135465727474174</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8080088392438437</v>
+        <v>0.8690609149157016</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8639517661142476</v>
+        <v>0.8546805378875918</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1688771773989653</v>
+        <v>3.008495282459621</v>
       </c>
       <c r="I12" t="n">
-        <v>5.035098001061732</v>
+        <v>0.0002841402764911615</v>
       </c>
       <c r="J12" t="n">
-        <v>0.07708450122108779</v>
+        <v>0.08278858782820846</v>
       </c>
       <c r="K12" t="n">
-        <v>0.7208930506374178</v>
+        <v>0.3969826479745209</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5988404090096581</v>
+        <v>0.02728677903593511</v>
       </c>
       <c r="M12" t="n">
-        <v>3.178063018034816</v>
+        <v>0.8516488109398002</v>
       </c>
       <c r="N12" t="n">
-        <v>0.000210588374111578</v>
+        <v>0.4832927027924745</v>
       </c>
       <c r="O12" t="n">
-        <v>0.5297222240549483</v>
+        <v>0.2153449809207874</v>
       </c>
       <c r="P12" t="n">
-        <v>3.054765979526099</v>
+        <v>4.562913200909448</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0004070837505172241</v>
+        <v>0.08108768343153451</v>
       </c>
       <c r="R12" t="n">
-        <v>0.07201775453291377</v>
+        <v>0.8902452024379236</v>
       </c>
       <c r="S12" t="n">
-        <v>0.4113222257540606</v>
+        <v>0.5757749501784661</v>
       </c>
       <c r="T12" t="n">
-        <v>0.03487843412975469</v>
+        <v>2.893161157922731</v>
       </c>
       <c r="U12" t="n">
-        <v>0.6653915060381269</v>
+        <v>0.0002852013679755379</v>
       </c>
       <c r="V12" t="n">
-        <v>0.5879602380139209</v>
+        <v>0.7441903469507021</v>
       </c>
       <c r="W12" t="n">
-        <v>0.9683926180428197</v>
+        <v>1.193721608611909</v>
       </c>
       <c r="X12" t="n">
-        <v>0.1257305979518778</v>
+        <v>0.1337207241315265</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.07531514860239402</v>
+        <v>0.06390819474209217</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.6409194378820665</v>
+        <v>0.5008462450805663</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.5509014734719482</v>
+        <v>0.6653137652650156</v>
       </c>
       <c r="AB12" t="n">
-        <v>-0.02748349172799392</v>
+        <v>-0.033792380764079</v>
       </c>
     </row>
     <row r="13">
@@ -1537,85 +1537,85 @@
         <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>327128.4958928578</v>
+        <v>329941.8896328636</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8382492599025628</v>
+        <v>0.8230866079480571</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8779311643208778</v>
+        <v>0.792987521133387</v>
       </c>
       <c r="E13" t="n">
-        <v>0.7891339039013583</v>
+        <v>0.8891479823339418</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7881762609225527</v>
+        <v>0.7909475413614198</v>
       </c>
       <c r="G13" t="n">
-        <v>0.8305552716354123</v>
+        <v>0.8239601482181073</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2071277234436282</v>
+        <v>2.821027705219672</v>
       </c>
       <c r="I13" t="n">
-        <v>5.129155527555976</v>
+        <v>0.0003836180034624139</v>
       </c>
       <c r="J13" t="n">
-        <v>0.08854211822729999</v>
+        <v>0.06405645886846445</v>
       </c>
       <c r="K13" t="n">
-        <v>0.7696943262730402</v>
+        <v>0.4762491372614564</v>
       </c>
       <c r="L13" t="n">
-        <v>0.6483108488841705</v>
+        <v>0.03444761711868893</v>
       </c>
       <c r="M13" t="n">
-        <v>3.119123006761815</v>
+        <v>0.8045716466799497</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0002576385568125622</v>
+        <v>0.5250248761441119</v>
       </c>
       <c r="O13" t="n">
-        <v>0.5701329133156279</v>
+        <v>0.1779872341832881</v>
       </c>
       <c r="P13" t="n">
-        <v>2.760348731546234</v>
+        <v>5.883951674890715</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.0002820110810685798</v>
+        <v>0.08374233303847782</v>
       </c>
       <c r="R13" t="n">
-        <v>0.06230672437513034</v>
+        <v>0.871458634845709</v>
       </c>
       <c r="S13" t="n">
-        <v>0.4226899759613774</v>
+        <v>0.6041304156583447</v>
       </c>
       <c r="T13" t="n">
-        <v>0.0366501638797765</v>
+        <v>3.04338130186395</v>
       </c>
       <c r="U13" t="n">
-        <v>0.7095541423678422</v>
+        <v>0.0002617693543126172</v>
       </c>
       <c r="V13" t="n">
-        <v>0.6361350939147404</v>
+        <v>0.6764872110567948</v>
       </c>
       <c r="W13" t="n">
-        <v>1.152796471063235</v>
+        <v>1.074460200212812</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1788329059053718</v>
+        <v>0.1904130765989664</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.06523058399538788</v>
+        <v>0.06510134783707239</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.6102706011950684</v>
+        <v>0.4613098626629383</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.5841774914568945</v>
+        <v>0.5186318032780892</v>
       </c>
       <c r="AB13" t="n">
-        <v>-0.03159388913947236</v>
+        <v>-0.02965796635266101</v>
       </c>
     </row>
   </sheetData>
@@ -1713,10 +1713,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.2212903992461807</v>
+        <v>-7.858230419450416</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.2212903992461807</v>
+        <v>-7.858230419450416</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1742,10 +1742,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.694329944638106</v>
+        <v>-0.3762006308260656</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.694329944638106</v>
+        <v>-0.3762006308260656</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -1771,10 +1771,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>-7.863637168322804</v>
+        <v>-0.3506449188426781</v>
       </c>
       <c r="C6" t="n">
-        <v>-7.863637168322804</v>
+        <v>-0.3506449188426781</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -1800,10 +1800,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>-7.867053400091845</v>
+        <v>-0.2814458373705803</v>
       </c>
       <c r="C7" t="n">
-        <v>-7.867053400091845</v>
+        <v>-0.2814458373705803</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>-7.858375398608628</v>
+        <v>-1.645332291627414</v>
       </c>
       <c r="C8" t="n">
-        <v>-7.858375398608628</v>
+        <v>-1.645332291627414</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -1858,10 +1858,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>-7.87398032592616</v>
+        <v>-1.948789242853682</v>
       </c>
       <c r="C9" t="n">
-        <v>-7.87398032592616</v>
+        <v>-1.948789242853682</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1887,10 +1887,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.877158370589198</v>
+        <v>-1.154423657579855</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.877158370589198</v>
+        <v>-1.154423657579855</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -1916,10 +1916,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.009719931284370781</v>
+        <v>-1.655692254147207</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.009719931284370781</v>
+        <v>-1.655692254147207</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -1945,10 +1945,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.05703991778956587</v>
+        <v>-0.2603155668458356</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.05703991778956587</v>
+        <v>-0.2603155668458356</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -1974,10 +1974,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.770874538212006</v>
+        <v>-0.1649870328555242</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.770874538212006</v>
+        <v>-0.1649870328555242</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -2091,10 +2091,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>-7.87398032592616</v>
+        <v>-7.858230419450416</v>
       </c>
       <c r="C4" t="n">
-        <v>-7.87398032592616</v>
+        <v>-7.858230419450416</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -2120,10 +2120,10 @@
         <v>0.05</v>
       </c>
       <c r="B5" t="n">
-        <v>-7.870863209300719</v>
+        <v>-5.198981889981885</v>
       </c>
       <c r="C5" t="n">
-        <v>-7.870863209300719</v>
+        <v>-5.198981889981885</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -2149,10 +2149,10 @@
         <v>0.25</v>
       </c>
       <c r="B6" t="n">
-        <v>-7.86232172589426</v>
+        <v>-1.653102263517259</v>
       </c>
       <c r="C6" t="n">
-        <v>-7.86232172589426</v>
+        <v>-1.653102263517259</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -2178,10 +2178,10 @@
         <v>0.5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.824016454400602</v>
+        <v>-0.7653121442029605</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.824016454400602</v>
+        <v>-0.7653121442029605</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -2207,10 +2207,10 @@
         <v>0.75</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.589550285594162</v>
+        <v>-0.2987456077386047</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.589550285594162</v>
+        <v>-0.2987456077386047</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -2236,10 +2236,10 @@
         <v>0.95</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.03101392521170862</v>
+        <v>-0.2078848731511645</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.03101392521170862</v>
+        <v>-0.2078848731511645</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -2265,10 +2265,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.009719931284370781</v>
+        <v>-0.1649870328555242</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.009719931284370781</v>
+        <v>-0.1649870328555242</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -2375,10 +2375,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.01818181818181818</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01818181818181818</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -2399,10 +2399,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.8303030303030302</v>
+        <v>0.1757575757575758</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.8303030303030302</v>
+        <v>0.1757575757575758</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
@@ -2419,10 +2419,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.2969696969696969</v>
+        <v>-0.2727272727272727</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2969696969696969</v>
+        <v>-0.2727272727272727</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
@@ -2443,10 +2443,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.6242424242424242</v>
+        <v>0.1151515151515151</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.6242424242424242</v>
+        <v>0.1151515151515151</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -2467,10 +2467,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.6848484848484848</v>
+        <v>0.1757575757575758</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6848484848484848</v>
+        <v>0.1757575757575758</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -2487,10 +2487,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.1151515151515151</v>
+        <v>-0.0303030303030303</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1151515151515151</v>
+        <v>-0.0303030303030303</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -2502,19 +2502,19 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Stream-s154</t>
+          <t>Stream-catalyst</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>S154 price [USD/kg]</t>
+          <t>Catalyst price [USD/kg]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1151515151515151</v>
+        <v>-0.5757575757575757</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1151515151515151</v>
+        <v>-0.5757575757575757</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
@@ -2526,19 +2526,19 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Stream-s155</t>
+          <t>Stream-biodiesel wash water</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>S155 price [USD/kg]</t>
+          <t>Biodiesel wash water price [USD/kg]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.09090909090909088</v>
+        <v>-0.4303030303030302</v>
       </c>
       <c r="D9" t="n">
-        <v>0.09090909090909088</v>
+        <v>-0.4303030303030302</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
@@ -2550,19 +2550,19 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Stream-lime</t>
+          <t>Stream-HCl</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>Lime price [USD/kg]</t>
+          <t>HCl price [USD/kg]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.3212121212121212</v>
+        <v>-0.3939393939393939</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3212121212121212</v>
+        <v>-0.3939393939393939</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -2574,19 +2574,19 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Stream-acetone</t>
+          <t>Stream-NaOH</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>Acetone price [USD/kg]</t>
+          <t>Na OH price [USD/kg]</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.3212121212121212</v>
+        <v>-0.1757575757575758</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3212121212121212</v>
+        <v>-0.1757575757575758</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
@@ -2598,19 +2598,19 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Stream-pure glycerine</t>
+          <t>Stream-oilcane</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Pure glycerine price [USD/kg]</t>
+          <t>Oilcane price [USD/kg]</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.4909090909090909</v>
+        <v>-0.4787878787878787</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.4909090909090909</v>
+        <v>-0.4787878787878787</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
@@ -2622,19 +2622,19 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Stream-cooling tower chemicals</t>
+          <t>Stream-denaturant</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>Cooling tower chemicals price [USD/kg]</t>
+          <t>Denaturant price [USD/kg]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.1393939393939394</v>
+        <v>0.1636363636363636</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.1393939393939394</v>
+        <v>0.1636363636363636</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
@@ -2646,19 +2646,19 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Stream-makeup water</t>
+          <t>Stream-methanol</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>Makeup water price [USD/kg]</t>
+          <t>Methanol price [USD/kg]</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.5636363636363636</v>
+        <v>-0.5757575757575757</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.5636363636363636</v>
+        <v>-0.5757575757575757</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
@@ -2670,19 +2670,19 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Stream-methanol</t>
+          <t>Stream-s154</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Methanol price [USD/kg]</t>
+          <t>S154 price [USD/kg]</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.04242424242424241</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.04242424242424241</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
@@ -2694,19 +2694,19 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Stream-catalyst</t>
+          <t>Stream-s155</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Catalyst price [USD/kg]</t>
+          <t>S155 price [USD/kg]</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.4181818181818182</v>
+        <v>-0.05454545454545454</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4181818181818182</v>
+        <v>-0.05454545454545454</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
@@ -2718,19 +2718,19 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Stream-biodiesel wash water</t>
+          <t>Stream-lime</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Biodiesel wash water price [USD/kg]</t>
+          <t>Lime price [USD/kg]</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.5757575757575757</v>
+        <v>0.0303030303030303</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5757575757575757</v>
+        <v>0.0303030303030303</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
@@ -2742,19 +2742,19 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Stream-HCl</t>
+          <t>Stream-acetone</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>HCl price [USD/kg]</t>
+          <t>Acetone price [USD/kg]</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5151515151515151</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
@@ -2766,19 +2766,19 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Stream-NaOH</t>
+          <t>Stream-pure glycerine</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Na OH price [USD/kg]</t>
+          <t>Pure glycerine price [USD/kg]</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.4303030303030302</v>
+        <v>-0.6242424242424242</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.4303030303030302</v>
+        <v>-0.6242424242424242</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
@@ -2790,19 +2790,19 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Stream-oilcane</t>
+          <t>Stream-cooling tower chemicals</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Oilcane price [USD/kg]</t>
+          <t>Cooling tower chemicals price [USD/kg]</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.1515151515151515</v>
+        <v>-0.5030303030303029</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.1515151515151515</v>
+        <v>-0.5030303030303029</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
@@ -2814,19 +2814,19 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Stream-denaturant</t>
+          <t>Stream-makeup water</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Denaturant price [USD/kg]</t>
+          <t>Makeup water price [USD/kg]</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.4424242424242424</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4424242424242424</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
@@ -2847,10 +2847,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.1272727272727273</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.1272727272727273</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
@@ -2871,10 +2871,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.4787878787878787</v>
+        <v>0.4424242424242424</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4787878787878787</v>
+        <v>0.4424242424242424</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
@@ -2895,10 +2895,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.2121212121212121</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.2121212121212121</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
@@ -2919,10 +2919,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.2121212121212121</v>
+        <v>-0.1878787878787879</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2121212121212121</v>
+        <v>-0.1878787878787879</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
@@ -2943,10 +2943,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.1636363636363636</v>
+        <v>-0.4545454545454545</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1636363636363636</v>
+        <v>-0.4545454545454545</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
@@ -2963,10 +2963,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-0.1515151515151515</v>
+        <v>-0.2121212121212121</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.1515151515151515</v>
+        <v>-0.2121212121212121</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
@@ -2987,10 +2987,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.07878787878787878</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.07878787878787878</v>
+        <v>0.05454545454545454</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -3053,72 +3053,72 @@
       <c r="G1" s="1" t="n"/>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Stream-catalyst</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-biodiesel wash water</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-HCl</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-NaOH</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-oilcane</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-denaturant</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Stream-methanol</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>Stream-s154</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Stream-s155</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Stream-lime</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Stream-acetone</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Stream-pure glycerine</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Stream-cooling tower chemicals</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Stream-makeup water</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-methanol</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-catalyst</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-biodiesel wash water</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-HCl</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-NaOH</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-oilcane</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Stream-denaturant</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
@@ -3203,72 +3203,72 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
+          <t>Catalyst price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Biodiesel wash water price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>HCl price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>Na OH price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>Oilcane price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>Denaturant price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>Methanol price [USD/kg]</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
           <t>S154 price [USD/kg]</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>S155 price [USD/kg]</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>Lime price [USD/kg]</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>Acetone price [USD/kg]</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="S2" s="1" t="inlineStr">
         <is>
           <t>Pure glycerine price [USD/kg]</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>Cooling tower chemicals price [USD/kg]</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>Makeup water price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>Methanol price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>Catalyst price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>Biodiesel wash water price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="R2" s="1" t="inlineStr">
-        <is>
-          <t>HCl price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="S2" s="1" t="inlineStr">
-        <is>
-          <t>Na OH price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="T2" s="1" t="inlineStr">
-        <is>
-          <t>Oilcane price [USD/kg]</t>
-        </is>
-      </c>
-      <c r="U2" s="1" t="inlineStr">
-        <is>
-          <t>Denaturant price [USD/kg]</t>
         </is>
       </c>
       <c r="V2" s="1" t="inlineStr">
@@ -3352,91 +3352,91 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>357932.6012637048</v>
+        <v>319933.8791364545</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8050793421093427</v>
+        <v>0.8786644138052185</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9473563265903202</v>
+        <v>0.8871937031661965</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7405554300604852</v>
+        <v>0.7547278197304041</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8177556382943275</v>
+        <v>0.8052815644220522</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8848171238933005</v>
+        <v>0.8489016030834337</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2304649160473426</v>
+        <v>3.371083913010652</v>
       </c>
       <c r="I4" t="n">
-        <v>4.018721223551006</v>
+        <v>0.0003606812768118197</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06687066685588682</v>
+        <v>0.07410749344466867</v>
       </c>
       <c r="K4" t="n">
-        <v>0.939339977825246</v>
+        <v>0.4552178678269928</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6707046980773463</v>
+        <v>0.0353641481148252</v>
       </c>
       <c r="M4" t="n">
-        <v>2.866617665688383</v>
+        <v>0.8826563199816162</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0002500360999305225</v>
+        <v>0.6522672418471019</v>
       </c>
       <c r="O4" t="n">
-        <v>0.6463647004946969</v>
+        <v>0.1959209426376695</v>
       </c>
       <c r="P4" t="n">
-        <v>2.77165469984371</v>
+        <v>5.470272573962804</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0004009528610403349</v>
+        <v>0.08649226948631465</v>
       </c>
       <c r="R4" t="n">
-        <v>0.0751299091857897</v>
+        <v>0.789789487261971</v>
       </c>
       <c r="S4" t="n">
-        <v>0.3446022514793721</v>
+        <v>0.7068668259051389</v>
       </c>
       <c r="T4" t="n">
-        <v>0.03273125844191845</v>
+        <v>3.40564778091172</v>
       </c>
       <c r="U4" t="n">
-        <v>0.7991714146296076</v>
+        <v>0.0002530966049521194</v>
       </c>
       <c r="V4" t="n">
-        <v>0.6878961757376787</v>
+        <v>0.6063536285641343</v>
       </c>
       <c r="W4" t="n">
-        <v>1.253519514243771</v>
+        <v>1.140441508435972</v>
       </c>
       <c r="X4" t="n">
-        <v>0.1707587393208577</v>
+        <v>0.1432311571221447</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.05698111291165429</v>
+        <v>0.07089763418581578</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.5780738828464115</v>
+        <v>0.6234441682918634</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.694883026479991</v>
+        <v>0.628306728617419</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.03688387115176386</v>
+        <v>-0.03191340379370473</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.2212903992461807</v>
+        <v>-7.858230419450416</v>
       </c>
       <c r="AD4" t="n">
-        <v>-0.2212903992461807</v>
+        <v>-7.858230419450416</v>
       </c>
       <c r="AE4" t="n">
         <v>0</v>
@@ -3462,91 +3462,91 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>380874.5579471973</v>
+        <v>313564.8105574455</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8848928661378663</v>
+        <v>0.7998684796327056</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6946711890489051</v>
+        <v>0.7244969015158683</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8840091028660189</v>
+        <v>0.8322339575776623</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8294670072924083</v>
+        <v>0.7999660034436795</v>
       </c>
       <c r="G5" t="n">
-        <v>0.84641421771937</v>
+        <v>0.8830702141683747</v>
       </c>
       <c r="H5" t="n">
-        <v>0.21422386968229</v>
+        <v>2.743042574648345</v>
       </c>
       <c r="I5" t="n">
-        <v>5.890321925513112</v>
+        <v>0.0003289364024939061</v>
       </c>
       <c r="J5" t="n">
-        <v>0.08299128037592571</v>
+        <v>0.07687303024649192</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9082071720196501</v>
+        <v>0.3300847609639892</v>
       </c>
       <c r="L5" t="n">
-        <v>0.6556124558378787</v>
+        <v>0.03220473282091099</v>
       </c>
       <c r="M5" t="n">
-        <v>3.067923688148006</v>
+        <v>0.6227138591153392</v>
       </c>
       <c r="N5" t="n">
-        <v>0.0002762051863299435</v>
+        <v>0.5403375284695384</v>
       </c>
       <c r="O5" t="n">
-        <v>0.6149568146394602</v>
+        <v>0.2189978976353245</v>
       </c>
       <c r="P5" t="n">
-        <v>3.505156157978153</v>
+        <v>4.878687567321744</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0003531316033044186</v>
+        <v>0.07119481577661639</v>
       </c>
       <c r="R5" t="n">
-        <v>0.07861538951185934</v>
+        <v>0.6684021898548804</v>
       </c>
       <c r="S5" t="n">
-        <v>0.3582513665714649</v>
+        <v>0.5583616497817865</v>
       </c>
       <c r="T5" t="n">
-        <v>0.03854801717921231</v>
+        <v>2.397484135322718</v>
       </c>
       <c r="U5" t="n">
-        <v>0.826881623507433</v>
+        <v>0.0002973096862628245</v>
       </c>
       <c r="V5" t="n">
-        <v>0.6126337564797641</v>
+        <v>0.6235737575200697</v>
       </c>
       <c r="W5" t="n">
-        <v>1.171157103863737</v>
+        <v>1.124533060291984</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1666614805182885</v>
+        <v>0.1617178972468668</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.06841455172905073</v>
+        <v>0.07677557266839527</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.4117509574256206</v>
+        <v>0.4296267132280529</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.6548330429996689</v>
+        <v>0.5633296252026652</v>
       </c>
       <c r="AB5" t="n">
-        <v>-0.02396246450497103</v>
+        <v>-0.03673171780419767</v>
       </c>
       <c r="AC5" t="n">
-        <v>-1.694329944638106</v>
+        <v>-0.3762006308260656</v>
       </c>
       <c r="AD5" t="n">
-        <v>-1.694329944638106</v>
+        <v>-0.3762006308260656</v>
       </c>
       <c r="AE5" t="n">
         <v>0</v>
@@ -3572,91 +3572,91 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>339464.7892672957</v>
+        <v>298652.536961208</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8749111178413539</v>
+        <v>0.913598896791175</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7116653946998395</v>
+        <v>0.943496240823478</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9517411438805221</v>
+        <v>0.9113945443861972</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7336412871831807</v>
+        <v>0.8367900742233263</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9063845158144797</v>
+        <v>0.9050128317595117</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2005501439903596</v>
+        <v>2.428895133991007</v>
       </c>
       <c r="I6" t="n">
-        <v>4.437146399598171</v>
+        <v>0.0003349395669201685</v>
       </c>
       <c r="J6" t="n">
-        <v>0.07672740599443309</v>
+        <v>0.06535896488265164</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6448483237247977</v>
+        <v>0.3718497468777013</v>
       </c>
       <c r="L6" t="n">
-        <v>0.6263909441650932</v>
+        <v>0.03077571193578649</v>
       </c>
       <c r="M6" t="n">
-        <v>2.539087679486212</v>
+        <v>0.7339930552387709</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0002352699943945606</v>
+        <v>0.5626895778130635</v>
       </c>
       <c r="O6" t="n">
-        <v>0.5812744007026547</v>
+        <v>0.1865517132625418</v>
       </c>
       <c r="P6" t="n">
-        <v>2.38668863019183</v>
+        <v>4.455897444275112</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.0003255906676568453</v>
+        <v>0.06673526631902278</v>
       </c>
       <c r="R6" t="n">
-        <v>0.07780260776090593</v>
+        <v>0.826143511831454</v>
       </c>
       <c r="S6" t="n">
-        <v>0.4693862935235245</v>
+        <v>0.7296670527853253</v>
       </c>
       <c r="T6" t="n">
-        <v>0.03240840898660156</v>
+        <v>2.921417212231451</v>
       </c>
       <c r="U6" t="n">
-        <v>0.7267467288232681</v>
+        <v>0.0002203378486013878</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7253610850711051</v>
+        <v>0.5711303623513122</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8611082579166746</v>
+        <v>1.337108941149416</v>
       </c>
       <c r="X6" t="n">
-        <v>0.157516751009419</v>
+        <v>0.1473001313631098</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.06067101652561339</v>
+        <v>0.04973075899074028</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.5903749241971649</v>
+        <v>0.4369975314761926</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.5215313297916584</v>
+        <v>0.5239575505479821</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.02533049424388528</v>
+        <v>-0.02503493230972102</v>
       </c>
       <c r="AC6" t="n">
-        <v>-7.863637168322804</v>
+        <v>-0.3506449188426781</v>
       </c>
       <c r="AD6" t="n">
-        <v>-7.863637168322804</v>
+        <v>-0.3506449188426781</v>
       </c>
       <c r="AE6" t="n">
         <v>0</v>
@@ -3682,91 +3682,91 @@
         <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>306651.6496836966</v>
+        <v>373253.3617076025</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9483675794212933</v>
+        <v>0.9615925260144773</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8662597510003653</v>
+        <v>0.9166889648538187</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8490271008094838</v>
+        <v>0.9486240135092125</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7742700633634951</v>
+        <v>0.7723284792010902</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8770973509454676</v>
+        <v>0.8183695922241495</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1892556229235258</v>
+        <v>2.888508906946005</v>
       </c>
       <c r="I7" t="n">
-        <v>5.304103991257275</v>
+        <v>0.0003521331319636663</v>
       </c>
       <c r="J7" t="n">
-        <v>0.08108096161014949</v>
+        <v>0.06149890043060448</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7906268219097432</v>
+        <v>0.4007447454966814</v>
       </c>
       <c r="L7" t="n">
-        <v>0.7049946873095743</v>
+        <v>0.03749849115362162</v>
       </c>
       <c r="M7" t="n">
-        <v>3.29781953084454</v>
+        <v>0.7371042881218192</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0002785990496345957</v>
+        <v>0.5539201297055767</v>
       </c>
       <c r="O7" t="n">
-        <v>0.5506236888700741</v>
+        <v>0.2006651951209002</v>
       </c>
       <c r="P7" t="n">
-        <v>2.535191236107107</v>
+        <v>5.17705000214424</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0003156966645211407</v>
+        <v>0.07554682695622253</v>
       </c>
       <c r="R7" t="n">
-        <v>0.06823077024195216</v>
+        <v>0.7072223399099908</v>
       </c>
       <c r="S7" t="n">
-        <v>0.3836085530734214</v>
+        <v>0.6250222003260829</v>
       </c>
       <c r="T7" t="n">
-        <v>0.04058299123724349</v>
+        <v>2.693368682757011</v>
       </c>
       <c r="U7" t="n">
-        <v>0.7785495170741203</v>
+        <v>0.0002432283270730846</v>
       </c>
       <c r="V7" t="n">
-        <v>0.702566135301615</v>
+        <v>0.6707481097186991</v>
       </c>
       <c r="W7" t="n">
-        <v>1.056249536722339</v>
+        <v>1.22594003824971</v>
       </c>
       <c r="X7" t="n">
-        <v>0.1480772555405145</v>
+        <v>0.1737448321091259</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.07186591905146845</v>
+        <v>0.06582908898554571</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.5490981127761296</v>
+        <v>0.6520917483703238</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.5634543443433764</v>
+        <v>0.614031479278348</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.03335754274654502</v>
+        <v>-0.03121978261009316</v>
       </c>
       <c r="AC7" t="n">
-        <v>-7.867053400091845</v>
+        <v>-0.2814458373705803</v>
       </c>
       <c r="AD7" t="n">
-        <v>-7.867053400091845</v>
+        <v>-0.2814458373705803</v>
       </c>
       <c r="AE7" t="n">
         <v>0</v>
@@ -3792,91 +3792,91 @@
         <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>262514.6472840727</v>
+        <v>281680.2219344516</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9776222478985327</v>
+        <v>0.9969116463250449</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7509482924711647</v>
+        <v>0.8595948980231926</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9255614997637419</v>
+        <v>0.7994477860400596</v>
       </c>
       <c r="F8" t="n">
-        <v>0.762761199003973</v>
+        <v>0.808929405160542</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8004565699820949</v>
+        <v>0.7915694994022243</v>
       </c>
       <c r="H8" t="n">
-        <v>0.222414628104058</v>
+        <v>2.965343095009235</v>
       </c>
       <c r="I8" t="n">
-        <v>4.858549629553575</v>
+        <v>0.0003698078739804615</v>
       </c>
       <c r="J8" t="n">
-        <v>0.07346495704723242</v>
+        <v>0.07060588205798324</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8383980380237968</v>
+        <v>0.3858916738723712</v>
       </c>
       <c r="L8" t="n">
-        <v>0.5013976616738217</v>
+        <v>0.03317278914125589</v>
       </c>
       <c r="M8" t="n">
-        <v>2.811651265696538</v>
+        <v>0.7709245333954597</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0002614183494726501</v>
+        <v>0.5072953946658069</v>
       </c>
       <c r="O8" t="n">
-        <v>0.5138991706686693</v>
+        <v>0.2478154060836067</v>
       </c>
       <c r="P8" t="n">
-        <v>3.223722110428652</v>
+        <v>4.154164732492569</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.000374478451998614</v>
+        <v>0.09144690280952712</v>
       </c>
       <c r="R8" t="n">
-        <v>0.07166848239099474</v>
+        <v>0.7463118804327451</v>
       </c>
       <c r="S8" t="n">
-        <v>0.4072027635374821</v>
+        <v>0.6565684310540738</v>
       </c>
       <c r="T8" t="n">
-        <v>0.02699802592531141</v>
+        <v>2.804626114575094</v>
       </c>
       <c r="U8" t="n">
-        <v>0.7653313531650924</v>
+        <v>0.000198263257584019</v>
       </c>
       <c r="V8" t="n">
-        <v>0.6677690295363166</v>
+        <v>0.7124049616723603</v>
       </c>
       <c r="W8" t="n">
-        <v>1.042586632760334</v>
+        <v>1.093486639699995</v>
       </c>
       <c r="X8" t="n">
-        <v>0.151808114866478</v>
+        <v>0.1652754070604397</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.05851927416908165</v>
+        <v>0.05914527682491581</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.444357116852826</v>
+        <v>0.5778473413310297</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.6767308840556633</v>
+        <v>0.6508017048837519</v>
       </c>
       <c r="AB8" t="n">
-        <v>-0.02665573302878534</v>
+        <v>-0.02602294793059929</v>
       </c>
       <c r="AC8" t="n">
-        <v>-7.858375398608628</v>
+        <v>-1.645332291627414</v>
       </c>
       <c r="AD8" t="n">
-        <v>-7.858375398608628</v>
+        <v>-1.645332291627414</v>
       </c>
       <c r="AE8" t="n">
         <v>0</v>
@@ -3902,91 +3902,91 @@
         <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>374835.9216336525</v>
+        <v>400402.9982207899</v>
       </c>
       <c r="C9" t="n">
-        <v>0.96345743369695</v>
+        <v>0.8443328418904813</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7976356757661157</v>
+        <v>0.7438957710474825</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8212491308656801</v>
+        <v>0.8594039968340557</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7981961958628567</v>
+        <v>0.7461817695488248</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8351630490737511</v>
+        <v>0.833700452055553</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1847439318249173</v>
+        <v>3.17804860258555</v>
       </c>
       <c r="I9" t="n">
-        <v>4.601013982454439</v>
+        <v>0.0003892960700962455</v>
       </c>
       <c r="J9" t="n">
-        <v>0.07005841816291634</v>
+        <v>0.07959573339432315</v>
       </c>
       <c r="K9" t="n">
-        <v>0.7541013758032719</v>
+        <v>0.4123240968521634</v>
       </c>
       <c r="L9" t="n">
-        <v>0.7597633661141168</v>
+        <v>0.0404902691028737</v>
       </c>
       <c r="M9" t="n">
-        <v>3.443838137939585</v>
+        <v>0.7124796148590791</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0002936131766009249</v>
+        <v>0.5831842329375594</v>
       </c>
       <c r="O9" t="n">
-        <v>0.4312023970755172</v>
+        <v>0.1928873412831012</v>
       </c>
       <c r="P9" t="n">
-        <v>2.938731695466159</v>
+        <v>5.416343020792297</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0003480708247751944</v>
+        <v>0.07344880365788668</v>
       </c>
       <c r="R9" t="n">
-        <v>0.06694034404471129</v>
+        <v>0.9156469590806386</v>
       </c>
       <c r="S9" t="n">
-        <v>0.4352197954596095</v>
+        <v>0.7550472805697284</v>
       </c>
       <c r="T9" t="n">
-        <v>0.03365331171496774</v>
+        <v>3.217569490505013</v>
       </c>
       <c r="U9" t="n">
-        <v>0.6153240920929001</v>
+        <v>0.0002313902238183701</v>
       </c>
       <c r="V9" t="n">
-        <v>0.5162034309052904</v>
+        <v>0.5121386256421967</v>
       </c>
       <c r="W9" t="n">
-        <v>1.108924586452716</v>
+        <v>0.9846438667994801</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1450744958004219</v>
+        <v>0.1546985354806635</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.06346109196674382</v>
+        <v>0.06807566730984353</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.4648285702398428</v>
+        <v>0.5410149077664257</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.6244501301952565</v>
+        <v>0.5964974973357967</v>
       </c>
       <c r="AB9" t="n">
-        <v>-0.0288528336010218</v>
+        <v>-0.0351770958973858</v>
       </c>
       <c r="AC9" t="n">
-        <v>-7.87398032592616</v>
+        <v>-1.948789242853682</v>
       </c>
       <c r="AD9" t="n">
-        <v>-7.87398032592616</v>
+        <v>-1.948789242853682</v>
       </c>
       <c r="AE9" t="n">
         <v>0</v>
@@ -4012,91 +4012,91 @@
         <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>319102.759530023</v>
+        <v>351175.8106339728</v>
       </c>
       <c r="C10" t="n">
-        <v>0.900334206541735</v>
+        <v>0.8697762383658201</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9917626146810653</v>
+        <v>0.8182754452483054</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9774766061836527</v>
+        <v>0.7013345707951792</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8206141369524137</v>
+        <v>0.7578739986428953</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8174669755169829</v>
+        <v>0.8593642329489898</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1749728632329005</v>
+        <v>2.638420686539074</v>
       </c>
       <c r="I10" t="n">
-        <v>5.640251850759157</v>
+        <v>0.0003196245252555553</v>
       </c>
       <c r="J10" t="n">
-        <v>0.06409775651586852</v>
+        <v>0.06894728972837243</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8506783990961555</v>
+        <v>0.4315126165352834</v>
       </c>
       <c r="L10" t="n">
-        <v>0.7207662411245863</v>
+        <v>0.03834731055504404</v>
       </c>
       <c r="M10" t="n">
-        <v>2.695074613041329</v>
+        <v>0.795378220251483</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0002271947735975387</v>
+        <v>0.4489860102373564</v>
       </c>
       <c r="O10" t="n">
-        <v>0.4739654241589719</v>
+        <v>0.2090332745895152</v>
       </c>
       <c r="P10" t="n">
-        <v>2.895101327008005</v>
+        <v>5.019382691916063</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.0003422122621223608</v>
+        <v>0.07707060939494925</v>
       </c>
       <c r="R10" t="n">
-        <v>0.05850898993652914</v>
+        <v>0.768428041134154</v>
       </c>
       <c r="S10" t="n">
-        <v>0.4567708065267042</v>
+        <v>0.6807928507109652</v>
       </c>
       <c r="T10" t="n">
-        <v>0.03611581549339146</v>
+        <v>3.492202002166365</v>
       </c>
       <c r="U10" t="n">
-        <v>0.7499256611090723</v>
+        <v>0.0002691924648784527</v>
       </c>
       <c r="V10" t="n">
-        <v>0.5712623011318159</v>
+        <v>0.5865003479315394</v>
       </c>
       <c r="W10" t="n">
-        <v>1.087289938140449</v>
+        <v>1.013203054986206</v>
       </c>
       <c r="X10" t="n">
-        <v>0.1850441239581416</v>
+        <v>0.1593809587985065</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.0526963008505729</v>
+        <v>0.05553158358841925</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.6933977555140731</v>
+        <v>0.5981087897930929</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.6060014142635686</v>
+        <v>0.6893331415071603</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.03480064746924984</v>
+        <v>-0.02393852033030601</v>
       </c>
       <c r="AC10" t="n">
-        <v>-1.877158370589198</v>
+        <v>-1.154423657579855</v>
       </c>
       <c r="AD10" t="n">
-        <v>-1.877158370589198</v>
+        <v>-1.154423657579855</v>
       </c>
       <c r="AE10" t="n">
         <v>0</v>
@@ -4122,91 +4122,91 @@
         <v>7</v>
       </c>
       <c r="B11" t="n">
-        <v>299040.5542209736</v>
+        <v>337659.3293759496</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7966365430890057</v>
+        <v>0.7736179346218206</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8348915746762982</v>
+        <v>0.9973860093723005</v>
       </c>
       <c r="E11" t="n">
-        <v>0.684490276926683</v>
+        <v>0.9972793057091298</v>
       </c>
       <c r="F11" t="n">
-        <v>0.867094504336779</v>
+        <v>0.8219447735447114</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8528564833821041</v>
+        <v>0.8747207804720781</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1958610414348189</v>
+        <v>3.240585565110913</v>
       </c>
       <c r="I11" t="n">
-        <v>4.884598240308491</v>
+        <v>0.0004200628429911011</v>
       </c>
       <c r="J11" t="n">
-        <v>0.08610130316578292</v>
+        <v>0.07327363422485261</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8002623188850734</v>
+        <v>0.4386008280703952</v>
       </c>
       <c r="L11" t="n">
-        <v>0.576485939601547</v>
+        <v>0.03594314236113292</v>
       </c>
       <c r="M11" t="n">
-        <v>2.93649508044741</v>
+        <v>0.662310983551104</v>
       </c>
       <c r="N11" t="n">
-        <v>0.000247186030009474</v>
+        <v>0.6024099123734256</v>
       </c>
       <c r="O11" t="n">
-        <v>0.5418198638264584</v>
+        <v>0.159822979639685</v>
       </c>
       <c r="P11" t="n">
-        <v>3.172639721840791</v>
+        <v>4.827616848356666</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0003715558475813992</v>
+        <v>0.06540690132546848</v>
       </c>
       <c r="R11" t="n">
-        <v>0.08536282500207992</v>
+        <v>0.8046943861715045</v>
       </c>
       <c r="S11" t="n">
-        <v>0.3950506301802912</v>
+        <v>0.6471059832167992</v>
       </c>
       <c r="T11" t="n">
-        <v>0.03063638760737266</v>
+        <v>3.116009606296744</v>
       </c>
       <c r="U11" t="n">
-        <v>0.8967484793597706</v>
+        <v>0.000254807598542642</v>
       </c>
       <c r="V11" t="n">
-        <v>0.6317349260299548</v>
+        <v>0.6400406371680076</v>
       </c>
       <c r="W11" t="n">
-        <v>1.285812441949361</v>
+        <v>0.8757355991885388</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1631159534491266</v>
+        <v>0.1802062198730517</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.06597089756153006</v>
+        <v>0.06237778198822949</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.5019972760358175</v>
+        <v>0.6796867243162839</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.517959691355853</v>
+        <v>0.5455972242559897</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.03016929260170088</v>
+        <v>-0.02764856853801772</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.009719931284370781</v>
+        <v>-1.655692254147207</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.009719931284370781</v>
+        <v>-1.655692254147207</v>
       </c>
       <c r="AE11" t="n">
         <v>0</v>
@@ -4232,91 +4232,91 @@
         <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>347404.9526774819</v>
+        <v>353922.3490579935</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7526196013002304</v>
+        <v>0.94378634000099</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9124882691678078</v>
+        <v>0.6941703842129278</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7255248407727003</v>
+        <v>0.7135465727474174</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8080088392438437</v>
+        <v>0.8690609149157016</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8639517661142476</v>
+        <v>0.8546805378875918</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1688771773989653</v>
+        <v>3.008495282459621</v>
       </c>
       <c r="I12" t="n">
-        <v>5.035098001061732</v>
+        <v>0.0002841402764911615</v>
       </c>
       <c r="J12" t="n">
-        <v>0.07708450122108779</v>
+        <v>0.08278858782820846</v>
       </c>
       <c r="K12" t="n">
-        <v>0.7208930506374178</v>
+        <v>0.3969826479745209</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5988404090096581</v>
+        <v>0.02728677903593511</v>
       </c>
       <c r="M12" t="n">
-        <v>3.178063018034816</v>
+        <v>0.8516488109398002</v>
       </c>
       <c r="N12" t="n">
-        <v>0.000210588374111578</v>
+        <v>0.4832927027924745</v>
       </c>
       <c r="O12" t="n">
-        <v>0.5297222240549483</v>
+        <v>0.2153449809207874</v>
       </c>
       <c r="P12" t="n">
-        <v>3.054765979526099</v>
+        <v>4.562913200909448</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0004070837505172241</v>
+        <v>0.08108768343153451</v>
       </c>
       <c r="R12" t="n">
-        <v>0.07201775453291377</v>
+        <v>0.8902452024379236</v>
       </c>
       <c r="S12" t="n">
-        <v>0.4113222257540606</v>
+        <v>0.5757749501784661</v>
       </c>
       <c r="T12" t="n">
-        <v>0.03487843412975469</v>
+        <v>2.893161157922731</v>
       </c>
       <c r="U12" t="n">
-        <v>0.6653915060381269</v>
+        <v>0.0002852013679755379</v>
       </c>
       <c r="V12" t="n">
-        <v>0.5879602380139209</v>
+        <v>0.7441903469507021</v>
       </c>
       <c r="W12" t="n">
-        <v>0.9683926180428197</v>
+        <v>1.193721608611909</v>
       </c>
       <c r="X12" t="n">
-        <v>0.1257305979518778</v>
+        <v>0.1337207241315265</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.07531514860239402</v>
+        <v>0.06390819474209217</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.6409194378820665</v>
+        <v>0.5008462450805663</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.5509014734719482</v>
+        <v>0.6653137652650156</v>
       </c>
       <c r="AB12" t="n">
-        <v>-0.02748349172799392</v>
+        <v>-0.033792380764079</v>
       </c>
       <c r="AC12" t="n">
-        <v>-0.05703991778956587</v>
+        <v>-0.2603155668458356</v>
       </c>
       <c r="AD12" t="n">
-        <v>-0.05703991778956587</v>
+        <v>-0.2603155668458356</v>
       </c>
       <c r="AE12" t="n">
         <v>0</v>
@@ -4342,91 +4342,91 @@
         <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>327128.4958928578</v>
+        <v>329941.8896328636</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8382492599025628</v>
+        <v>0.8230866079480571</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8779311643208778</v>
+        <v>0.792987521133387</v>
       </c>
       <c r="E13" t="n">
-        <v>0.7891339039013583</v>
+        <v>0.8891479823339418</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7881762609225527</v>
+        <v>0.7909475413614198</v>
       </c>
       <c r="G13" t="n">
-        <v>0.8305552716354123</v>
+        <v>0.8239601482181073</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2071277234436282</v>
+        <v>2.821027705219672</v>
       </c>
       <c r="I13" t="n">
-        <v>5.129155527555976</v>
+        <v>0.0003836180034624139</v>
       </c>
       <c r="J13" t="n">
-        <v>0.08854211822729999</v>
+        <v>0.06405645886846445</v>
       </c>
       <c r="K13" t="n">
-        <v>0.7696943262730402</v>
+        <v>0.4762491372614564</v>
       </c>
       <c r="L13" t="n">
-        <v>0.6483108488841705</v>
+        <v>0.03444761711868893</v>
       </c>
       <c r="M13" t="n">
-        <v>3.119123006761815</v>
+        <v>0.8045716466799497</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0002576385568125622</v>
+        <v>0.5250248761441119</v>
       </c>
       <c r="O13" t="n">
-        <v>0.5701329133156279</v>
+        <v>0.1779872341832881</v>
       </c>
       <c r="P13" t="n">
-        <v>2.760348731546234</v>
+        <v>5.883951674890715</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.0002820110810685798</v>
+        <v>0.08374233303847782</v>
       </c>
       <c r="R13" t="n">
-        <v>0.06230672437513034</v>
+        <v>0.871458634845709</v>
       </c>
       <c r="S13" t="n">
-        <v>0.4226899759613774</v>
+        <v>0.6041304156583447</v>
       </c>
       <c r="T13" t="n">
-        <v>0.0366501638797765</v>
+        <v>3.04338130186395</v>
       </c>
       <c r="U13" t="n">
-        <v>0.7095541423678422</v>
+        <v>0.0002617693543126172</v>
       </c>
       <c r="V13" t="n">
-        <v>0.6361350939147404</v>
+        <v>0.6764872110567948</v>
       </c>
       <c r="W13" t="n">
-        <v>1.152796471063235</v>
+        <v>1.074460200212812</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1788329059053718</v>
+        <v>0.1904130765989664</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.06523058399538788</v>
+        <v>0.06510134783707239</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.6102706011950684</v>
+        <v>0.4613098626629383</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.5841774914568945</v>
+        <v>0.5186318032780892</v>
       </c>
       <c r="AB13" t="n">
-        <v>-0.03159388913947236</v>
+        <v>-0.02965796635266101</v>
       </c>
       <c r="AC13" t="n">
-        <v>-1.770874538212006</v>
+        <v>-0.1649870328555242</v>
       </c>
       <c r="AD13" t="n">
-        <v>-1.770874538212006</v>
+        <v>-0.1649870328555242</v>
       </c>
       <c r="AE13" t="n">
         <v>0</v>

</xml_diff>